<commit_message>
Major Improvements to Iteration
- Removed milliseconds from timestamp
- Code now combines minutes + Hours
- Found and fixed a bug that cause renaming NA rows to cause all rows to become NA in Manual.ID column.
</commit_message>
<xml_diff>
--- a/Excels/Species Translations.xlsx
+++ b/Excels/Species Translations.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usceduau-my.sharepoint.com/personal/r_r113_student_usc_edu_au/Documents/Weather Model Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Bat Data\Bat Data\BatData\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{1D0E7AD1-51D2-4DBC-8266-D8E78E7B4E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{159E3499-2B17-41D8-B19A-5D8DD13B99AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D78C3B-AF0D-46A0-8AC7-833A5B5D004D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D88DE785-C7DC-449E-A9CD-C68FCE62A84F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D88DE785-C7DC-449E-A9CD-C68FCE62A84F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Species_Translations" sheetId="1" r:id="rId1"/>
+    <sheet name="Unknown_Translations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
-  <si>
-    <t>Ozimops ridei</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t xml:space="preserve">Austronomus australis </t>
   </si>
@@ -196,6 +194,27 @@
   </si>
   <si>
     <t>Myotis macropus</t>
+  </si>
+  <si>
+    <t>Unindentified Call</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Long eared bat</t>
+  </si>
+  <si>
+    <t>Little Goulds</t>
+  </si>
+  <si>
+    <t>Little?</t>
+  </si>
+  <si>
+    <t>Manual.ID</t>
+  </si>
+  <si>
+    <t>Translation</t>
   </si>
 </sst>
 </file>
@@ -266,9 +285,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,7 +325,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -412,7 +431,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,7 +573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -562,213 +581,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4743ABB-F903-406E-B994-A27267405BDF}">
-  <dimension ref="A2:Q10"/>
+  <dimension ref="A2:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
       <c r="F3">
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
         <v>28</v>
-      </c>
-      <c r="O3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
       </c>
       <c r="G7">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G10">
         <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A183F707-2634-4C9B-8BC5-96AAA696F9F9}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>